<commit_message>
working on network generation
</commit_message>
<xml_diff>
--- a/Network Models/Models 1-5 Scenario F Sim 3.xlsx
+++ b/Network Models/Models 1-5 Scenario F Sim 3.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jess/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jess/git/economic-model/Network Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F862E30-DDF8-C446-9664-DFB2355B3C7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1531CFE0-B922-B446-B4AD-A0506F1C321E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="6020" windowWidth="33260" windowHeight="16360" xr2:uid="{A6D17BEB-81C9-2541-ADAD-D79D704548F6}"/>
+    <workbookView xWindow="7180" yWindow="2800" windowWidth="40340" windowHeight="16440" xr2:uid="{A6D17BEB-81C9-2541-ADAD-D79D704548F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Hybrid SN=1 FN=101 T=50 A=0</t>
   </si>
   <si>
-    <t>PA SN=10 EN=100 T=19</t>
-  </si>
-  <si>
     <t>Complete Graph</t>
   </si>
   <si>
@@ -85,6 +82,30 @@
   </si>
   <si>
     <t>No Seller</t>
+  </si>
+  <si>
+    <t>V1.1</t>
+  </si>
+  <si>
+    <t>V1.2</t>
+  </si>
+  <si>
+    <t>Hybrid SN=10 EN=100 T=9 A=0</t>
+  </si>
+  <si>
+    <t>Hybrid SN=1   EN=101 T=99 A=0</t>
+  </si>
+  <si>
+    <t>Hybrid SN=2   EN=100 T=49 A=0</t>
+  </si>
+  <si>
+    <t>Hybrid SN=5   EN=100 T=19 A=0</t>
+  </si>
+  <si>
+    <t>New Generations</t>
+  </si>
+  <si>
+    <t>Prior Generations</t>
   </si>
 </sst>
 </file>
@@ -92,7 +113,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -150,7 +171,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -467,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7360BA8F-F7FE-2942-A550-D383E3D8D7DA}">
-  <dimension ref="B6:N12"/>
+  <dimension ref="A6:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -480,12 +501,15 @@
     <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
       <c r="K6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
@@ -514,16 +538,19 @@
         <v>7</v>
       </c>
       <c r="K7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="M7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>11</v>
       </c>
@@ -566,7 +593,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
@@ -609,7 +639,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -652,40 +685,41 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>12</v>
       </c>
       <c r="C11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D11">
-        <v>19.559999999999999</v>
+        <v>100</v>
       </c>
       <c r="E11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F11">
-        <v>1.82</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>0.34399999999999997</v>
+        <v>1</v>
       </c>
       <c r="H11">
         <v>100</v>
       </c>
       <c r="I11">
-        <v>978</v>
+        <f>100*99/2</f>
+        <v>4950</v>
       </c>
       <c r="J11" s="3">
         <f>(2*I11)/(H10*(H10-1))</f>
-        <v>0.19757575757575757</v>
+        <v>1</v>
       </c>
       <c r="K11" s="3">
-        <v>0.95679999999999998</v>
+        <v>1</v>
       </c>
       <c r="L11" s="3">
-        <v>4.3200000000000002E-2</v>
+        <v>0</v>
       </c>
       <c r="M11" s="3">
         <v>0</v>
@@ -695,47 +729,277 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12">
+      <c r="L14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1.98</v>
+      </c>
+      <c r="E15">
+        <v>12</v>
+      </c>
+      <c r="F15">
+        <v>5.4</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>100</v>
+      </c>
+      <c r="I15">
+        <v>99</v>
+      </c>
+      <c r="J15" s="3">
+        <f>(2*H15)/(I15*(I15-1))</f>
+        <v>2.0614306328592041E-2</v>
+      </c>
+      <c r="K15" s="3">
+        <v>0</v>
+      </c>
+      <c r="L15" s="3">
+        <v>0</v>
+      </c>
+      <c r="M15" s="3">
+        <v>0</v>
+      </c>
+      <c r="N15" s="2">
+        <f>SUM(K15:M15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>3.94</v>
+      </c>
+      <c r="E16">
+        <v>6</v>
+      </c>
+      <c r="F16">
+        <v>2.95</v>
+      </c>
+      <c r="G16">
+        <v>0.17</v>
+      </c>
+      <c r="H16">
+        <v>100</v>
+      </c>
+      <c r="I16">
+        <v>197</v>
+      </c>
+      <c r="J16" s="3">
+        <f>(2*I16)/(H15*(H15-1))</f>
+        <v>3.9797979797979798E-2</v>
+      </c>
+      <c r="K16" s="3">
+        <v>0</v>
+      </c>
+      <c r="L16" s="3">
+        <v>0</v>
+      </c>
+      <c r="M16" s="3">
+        <v>0</v>
+      </c>
+      <c r="N16" s="2">
+        <f>SUM(K16:M16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G17">
+        <v>0.22</v>
+      </c>
+      <c r="H17">
+        <v>100</v>
+      </c>
+      <c r="I17">
+        <v>485</v>
+      </c>
+      <c r="J17" s="3">
+        <f>(2*I17)/(H16*(H16-1))</f>
+        <v>9.7979797979797986E-2</v>
+      </c>
+      <c r="K17" s="3">
+        <v>0</v>
+      </c>
+      <c r="L17" s="3">
+        <v>0</v>
+      </c>
+      <c r="M17" s="3">
+        <v>0</v>
+      </c>
+      <c r="N17" s="2">
+        <f>SUM(K17:M17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <v>1.8</v>
+      </c>
+      <c r="G18">
+        <v>0.35</v>
+      </c>
+      <c r="H18">
+        <v>100</v>
+      </c>
+      <c r="I18">
+        <v>945</v>
+      </c>
+      <c r="J18" s="3">
+        <f>(2*I18)/(H17*(H17-1))</f>
+        <v>0.19090909090909092</v>
+      </c>
+      <c r="K18" s="3">
+        <v>0</v>
+      </c>
+      <c r="L18" s="3">
+        <v>0</v>
+      </c>
+      <c r="M18" s="3">
+        <v>0</v>
+      </c>
+      <c r="N18" s="2">
+        <f>SUM(K18:M18)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19">
         <v>5</v>
       </c>
-      <c r="D12">
+      <c r="D19">
         <v>100</v>
       </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
         <v>100</v>
       </c>
-      <c r="I12">
+      <c r="I19">
         <f>100*99/2</f>
         <v>4950</v>
       </c>
-      <c r="J12" s="3">
-        <f>(2*I12)/(H11*(H11-1))</f>
-        <v>1</v>
-      </c>
-      <c r="K12" s="3">
-        <v>1</v>
-      </c>
-      <c r="L12" s="3">
-        <v>0</v>
-      </c>
-      <c r="M12" s="3">
-        <v>0</v>
-      </c>
-      <c r="N12" s="2">
-        <f>SUM(K12:M12)</f>
+      <c r="J19" s="3">
+        <f>(2*I19)/(H17*(H17-1))</f>
+        <v>1</v>
+      </c>
+      <c r="K19" s="3">
+        <v>1</v>
+      </c>
+      <c r="L19" s="3">
+        <v>0</v>
+      </c>
+      <c r="M19" s="3">
+        <v>0</v>
+      </c>
+      <c r="N19" s="2">
+        <f>SUM(K19:M19)</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated hybrid network generation (output), ran simulations with new versions of models 1-4
</commit_message>
<xml_diff>
--- a/Network Models/Models 1-5 Scenario F Sim 3.xlsx
+++ b/Network Models/Models 1-5 Scenario F Sim 3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jess/git/economic-model/Network Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1531CFE0-B922-B446-B4AD-A0506F1C321E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B46FD92-F5C2-EB4E-B20D-7E56B448DF96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7180" yWindow="2800" windowWidth="40340" windowHeight="16440" xr2:uid="{A6D17BEB-81C9-2541-ADAD-D79D704548F6}"/>
+    <workbookView xWindow="4420" yWindow="15120" windowWidth="40340" windowHeight="16440" xr2:uid="{A6D17BEB-81C9-2541-ADAD-D79D704548F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -490,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7360BA8F-F7FE-2942-A550-D383E3D8D7DA}">
   <dimension ref="A6:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -808,17 +808,17 @@
         <v>2.0614306328592041E-2</v>
       </c>
       <c r="K15" s="3">
-        <v>0</v>
+        <v>0.23039999999999999</v>
       </c>
       <c r="L15" s="3">
-        <v>0</v>
+        <v>0.61560000000000004</v>
       </c>
       <c r="M15" s="3">
-        <v>0</v>
+        <v>0.15390000000000001</v>
       </c>
       <c r="N15" s="2">
         <f>SUM(K15:M15)</f>
-        <v>0</v>
+        <v>0.99990000000000012</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -854,17 +854,17 @@
         <v>3.9797979797979798E-2</v>
       </c>
       <c r="K16" s="3">
-        <v>0</v>
+        <v>0.3054</v>
       </c>
       <c r="L16" s="3">
-        <v>0</v>
+        <v>0.6946</v>
       </c>
       <c r="M16" s="3">
         <v>0</v>
       </c>
       <c r="N16" s="2">
         <f>SUM(K16:M16)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
@@ -900,17 +900,17 @@
         <v>9.7979797979797986E-2</v>
       </c>
       <c r="K17" s="3">
-        <v>0</v>
+        <v>0.70809999999999995</v>
       </c>
       <c r="L17" s="3">
-        <v>0</v>
+        <v>0.29189999999999999</v>
       </c>
       <c r="M17" s="3">
         <v>0</v>
       </c>
       <c r="N17" s="2">
         <f>SUM(K17:M17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
@@ -946,17 +946,17 @@
         <v>0.19090909090909092</v>
       </c>
       <c r="K18" s="3">
-        <v>0</v>
+        <v>0.94069999999999998</v>
       </c>
       <c r="L18" s="3">
-        <v>0</v>
+        <v>5.9299999999999999E-2</v>
       </c>
       <c r="M18" s="3">
         <v>0</v>
       </c>
       <c r="N18" s="2">
         <f>SUM(K18:M18)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
adding addtional simulation results
</commit_message>
<xml_diff>
--- a/Network Models/Models 1-5 Scenario F Sim 3.xlsx
+++ b/Network Models/Models 1-5 Scenario F Sim 3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jess/git/economic-model/Network Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B46FD92-F5C2-EB4E-B20D-7E56B448DF96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15359C4-4147-A847-BD48-EC0C61ECEFC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4420" yWindow="15120" windowWidth="40340" windowHeight="16440" xr2:uid="{A6D17BEB-81C9-2541-ADAD-D79D704548F6}"/>
+    <workbookView xWindow="3760" yWindow="10180" windowWidth="40340" windowHeight="16440" xr2:uid="{A6D17BEB-81C9-2541-ADAD-D79D704548F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t>Prior Generations</t>
+  </si>
+  <si>
+    <t>Scenario E, 5% sellers, TD=3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
   </si>
 </sst>
 </file>
@@ -488,10 +497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7360BA8F-F7FE-2942-A550-D383E3D8D7DA}">
-  <dimension ref="A6:N19"/>
+  <dimension ref="A6:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1003,6 +1012,109 @@
         <v>1</v>
       </c>
     </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J23" t="s">
+        <v>26</v>
+      </c>
+      <c r="K23" s="3">
+        <v>0.108</v>
+      </c>
+      <c r="L23" s="3">
+        <v>0.53680000000000005</v>
+      </c>
+      <c r="M23" s="3">
+        <v>0.3553</v>
+      </c>
+      <c r="N23" s="2">
+        <f>SUM(K23:M23)</f>
+        <v>1.0001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J24" t="s">
+        <v>26</v>
+      </c>
+      <c r="K24" s="3">
+        <v>0.21210000000000001</v>
+      </c>
+      <c r="L24" s="3">
+        <v>0.78059999999999996</v>
+      </c>
+      <c r="M24" s="3">
+        <v>7.1999999999999998E-3</v>
+      </c>
+      <c r="N24" s="2">
+        <f>SUM(K24:M24)</f>
+        <v>0.9998999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J25" t="s">
+        <v>27</v>
+      </c>
+      <c r="K25" s="3">
+        <v>0.4486</v>
+      </c>
+      <c r="L25" s="3">
+        <v>0.5514</v>
+      </c>
+      <c r="M25" s="3">
+        <v>0</v>
+      </c>
+      <c r="N25" s="2">
+        <f>SUM(K25:M25)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J26" t="s">
+        <v>26</v>
+      </c>
+      <c r="K26" s="3">
+        <v>0.67530000000000001</v>
+      </c>
+      <c r="L26" s="3">
+        <v>0.32469999999999999</v>
+      </c>
+      <c r="M26" s="3">
+        <v>0</v>
+      </c>
+      <c r="N26" s="2">
+        <f>SUM(K26:M26)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K27" s="3">
+        <v>1</v>
+      </c>
+      <c r="L27" s="3">
+        <v>0</v>
+      </c>
+      <c r="M27" s="3">
+        <v>0</v>
+      </c>
+      <c r="N27" s="2">
+        <f>SUM(K27:M27)</f>
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
supporting documents for blogging, new simulations
</commit_message>
<xml_diff>
--- a/Network Models/Models 1-5 Scenario F Sim 3.xlsx
+++ b/Network Models/Models 1-5 Scenario F Sim 3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jess/git/economic-model/Network Models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B9EC5FD-0A95-6348-8E99-66F8B59FC99B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F396A1-4708-2640-8EEB-DA7DE6692B87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3760" yWindow="10180" windowWidth="40340" windowHeight="16440" xr2:uid="{A6D17BEB-81C9-2541-ADAD-D79D704548F6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
   <si>
     <t>Name</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Scenario E, 10% sellers, TD=3</t>
   </si>
 </sst>
 </file>
@@ -499,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7360BA8F-F7FE-2942-A550-D383E3D8D7DA}">
   <dimension ref="A6:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1013,11 +1016,23 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>28</v>
+      </c>
       <c r="K21" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="K22" s="1" t="s">
         <v>13</v>
       </c>
@@ -1029,6 +1044,19 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F23" s="3">
+        <v>0</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0</v>
+      </c>
+      <c r="H23" s="3">
+        <v>0</v>
+      </c>
+      <c r="I23" s="2">
+        <f>SUM(F23:H23)</f>
+        <v>0</v>
+      </c>
       <c r="J23" t="s">
         <v>26</v>
       </c>
@@ -1047,6 +1075,19 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F24" s="3">
+        <v>0</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0</v>
+      </c>
+      <c r="I24" s="2">
+        <f>SUM(F24:H24)</f>
+        <v>0</v>
+      </c>
       <c r="J24" t="s">
         <v>26</v>
       </c>
@@ -1065,6 +1106,19 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F25" s="3">
+        <v>0</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0</v>
+      </c>
+      <c r="I25" s="2">
+        <f>SUM(F25:H25)</f>
+        <v>0</v>
+      </c>
       <c r="J25" t="s">
         <v>27</v>
       </c>
@@ -1083,6 +1137,19 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F26" s="3">
+        <v>0</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0</v>
+      </c>
+      <c r="H26" s="3">
+        <v>0</v>
+      </c>
+      <c r="I26" s="2">
+        <f>SUM(F26:H26)</f>
+        <v>0</v>
+      </c>
       <c r="J26" t="s">
         <v>26</v>
       </c>
@@ -1101,6 +1168,19 @@
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F27" s="3">
+        <v>1</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0</v>
+      </c>
+      <c r="H27" s="3">
+        <v>0</v>
+      </c>
+      <c r="I27" s="2">
+        <f>SUM(F27:H27)</f>
+        <v>1</v>
+      </c>
       <c r="K27" s="3">
         <v>1</v>
       </c>

</xml_diff>